<commit_message>
Updated Figures for HLA Revisions, coverage plots.py
</commit_message>
<xml_diff>
--- a/Results/Individual Results Australia.xlsx
+++ b/Results/Individual Results Australia.xlsx
@@ -7,16 +7,16 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Frequency" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Ebola GP1 (Zaire)" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Ebola GP1 (Sudan)" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Ebola NP (Zaire)" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Ebola NP (Sudan)" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Zaire Ebola GP" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sudan Ebola GP" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Zaire Ebola NP" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sudan Ebola NP" sheetId="5" state="visible" r:id="rId5"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SARS-CoV-2 Wuhan-Hu-1" sheetId="6" state="visible" r:id="rId6"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SARS-CoV-2 Delta AY.4" sheetId="7" state="visible" r:id="rId7"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SARS-CoV-2 Omicron BA.1" sheetId="8" state="visible" r:id="rId8"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SARS-CoV-2 Omicron BA.2" sheetId="9" state="visible" r:id="rId9"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="SARS-CoV-2 Omicron BA.5" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Burkholderia HCP1" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Burkholderia Hcp1" sheetId="11" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>

</xml_diff>